<commit_message>
updated python scripts for parsing of information
</commit_message>
<xml_diff>
--- a/assets/news/results/qualiperf_statistics.xlsx
+++ b/assets/news/results/qualiperf_statistics.xlsx
@@ -676,11 +676,7 @@
           <t>P6 - Reichenbach, P7 Ricken, P9 - Tautenhahn, Coordination</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr">
         <is>
           <t xml:space="preserve">10.1007/s00419-021-01907-3 </t>
@@ -816,11 +812,7 @@
           <t>P7 - Ricken, Coordination</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr">
         <is>
           <t>10.1002/pamm.202100190</t>
@@ -910,11 +902,7 @@
           <t>P7 - Ricken</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr">
         <is>
           <t>10.1016/j.ijsolstr.2021.111412</t>
@@ -1099,11 +1087,7 @@
           <t>P1 - Christ, P2 - Dahmen, P3 - König, P4 - Marz, P5 - Radde, P6 - Reichenbach, P7 - Ricken, P8 - Schwen, P9 - Tautenhahn, Coordination</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr">
         <is>
           <t>-</t>
@@ -1333,11 +1317,7 @@
           <t>P5 - Radde</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr">
         <is>
           <t>10.1016/j.ifacol.2023.01.020</t>
@@ -1474,11 +1454,7 @@
           <t>P7 - Ricken</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="H20" t="inlineStr"/>
       <c r="I20" t="inlineStr">
         <is>
           <t>10.1016/j.exco.2022.100087</t>
@@ -1618,11 +1594,7 @@
           <t>P7 - Ricken</t>
         </is>
       </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="H23" t="inlineStr"/>
       <c r="I23" t="inlineStr">
         <is>
           <t>10.3390/w15010159</t>
@@ -1668,11 +1640,7 @@
           <t>P7 - Ricken</t>
         </is>
       </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr">
         <is>
           <t>10.3390/w15020343</t>
@@ -2238,11 +2206,7 @@
           <t>P3 - König</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
           <t>10.20944/preprints202108.0303.v1</t>
@@ -2316,11 +2280,7 @@
           <t>P3 - König</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr">
         <is>
           <t xml:space="preserve"> 10.20944/preprints202108.0259.v1</t>
@@ -2470,11 +2430,7 @@
           <t>P3 - König</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr">
         <is>
           <t>10.48550/arXiv.2106.00844</t>
@@ -2549,11 +2505,7 @@
           <t>P3 - König</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
         <is>
           <t>10.1101/245076</t>
@@ -2589,11 +2541,7 @@
           <t>P3 - König</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr">
         <is>
           <t>10.20944/preprints202206.0137.v1</t>
@@ -2667,11 +2615,7 @@
           <t>P3 - König, P9 - Tautenhahn</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr">
         <is>
           <t>10.1101/2023.02.01.23285358</t>
@@ -2745,11 +2689,7 @@
           <t>P3 - König</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr">
         <is>
           <t>10.1101/2023.03.21.512712</t>
@@ -2787,11 +2727,7 @@
           <t>P3 - König, P9 - Tautenhahn</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr">
         <is>
           <t>10.1101/2023.04.12.536571</t>
@@ -2829,12 +2765,12 @@
           <t>P3 - König</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t xml:space="preserve">We present 11 strategies for making </t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>10.31219/osf.io/kcvra</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">

</xml_diff>

<commit_message>
changes for overview table
</commit_message>
<xml_diff>
--- a/assets/news/results/qualiperf_statistics.xlsx
+++ b/assets/news/results/qualiperf_statistics.xlsx
@@ -1171,8 +1171,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>J Integr Bioinform. 2021 Oct 22;18(3):20210026. doi: 10.1515/jib-2021-0026. PMID: 34674411; PMCID: PMC8573232.
-https://doi.org/10.1515/jib-2021-0026</t>
+          <t>J Integr Bioinform. 2021 Oct 22;18(3):20210026. doi: 10.1515/jib-2021-0026. PMID: 34674411; PMCID: PMC8573232. https://doi.org/10.1515/jib-2021-0026</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -1317,8 +1316,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Streptozotocin-Induced Diabetes Causes Changes in
-Serotonin-Positive Neurons in the Small Intestine in Pig Model</t>
+          <t>Streptozotocin-Induced Diabetes Causes Changes in Serotonin-Positive Neurons in the Small Intestine in Pig Model</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1684,8 +1682,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Examples and Counterexamples, 
-https://doi.org/10.1016/j.exco.2022.100087</t>
+          <t>Examples and Counterexamples,  https://doi.org/10.1016/j.exco.2022.100087</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -1775,8 +1772,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t xml:space="preserve">Periportal steatosis in mice affects distinct parameters of pericentral drug metabolism
-</t>
+          <t xml:space="preserve">Periportal steatosis in mice affects distinct parameters of pericentral drug metabolism </t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1827,9 +1823,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Uncertainty with Varying Subsurface Permeabilities Reduced
-Using Coupled Random Field and Extended Theory of Porous
-Media Contaminant Transport Models</t>
+          <t>Uncertainty with Varying Subsurface Permeabilities Reduced Using Coupled Random Field and Extended Theory of Porous Media Contaminant Transport Models</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1879,9 +1873,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Simulation of Contaminant Transport through the Vadose Zone:
-A Continuum Mechanical Approach within the Framework of
-the Extended Theory of Porous Media (eTPM)</t>
+          <t>Simulation of Contaminant Transport through the Vadose Zone: A Continuum Mechanical Approach within the Framework of the Extended Theory of Porous Media (eTPM)</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1981,9 +1973,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Critical Evaluation of Discarded Donor Livers 
-in the Eurotransplant Region: Potential 
-Implications for Machine Perfusion</t>
+          <t>Critical Evaluation of Discarded Donor Livers  in the Eurotransplant Region: Potential  Implications for Machine Perfusion</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1993,9 +1983,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>e-ISSN 2329-0358
-© Ann Transplant, 2023; 28: e938132
-DOI: 10.12659/AOT.938132</t>
+          <t>e-ISSN 2329-0358 © Ann Transplant, 2023; 28: e938132 DOI: 10.12659/AOT.938132</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -4072,8 +4060,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Fast 3D Isotropic High-Resolution MRI of Mouse Brain Using a Variable Flip Angle RARE
-Sequence With T2 Compensation @9.4T</t>
+          <t>Fast 3D Isotropic High-Resolution MRI of Mouse Brain Using a Variable Flip Angle RARE Sequence With T2 Compensation @9.4T</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -4462,8 +4449,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Bayesian estimation shows the merits of reproducible and reusable modeling in systems
-biology</t>
+          <t>Bayesian estimation shows the merits of reproducible and reusable modeling in systems biology</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -4673,8 +4659,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Multiscale and Multiphase Modeling of Function-Perfusion Processes in the Liver
-on Organ, Lobule and Cell Scale</t>
+          <t>Multiscale and Multiphase Modeling of Function-Perfusion Processes in the Liver on Organ, Lobule and Cell Scale</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -4892,9 +4877,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Simulation Supported Liver Assessment for Donor Organs (SimLivA) - Con-
-tinuum-Biomechanical Modeling for Staging of Ischemia Reperfusion Injury
-During Liver Transplantation</t>
+          <t>Simulation Supported Liver Assessment for Donor Organs (SimLivA) - Con- tinuum-Biomechanical Modeling for Staging of Ischemia Reperfusion Injury During Liver Transplantation</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -5162,17 +5145,17 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Category</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Title</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Authors</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Journal</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -5194,17 +5177,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>Editoring</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>Computational Modeling for Liver Surgery and Interventions</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>Bruno Christ, Uta Dahmen, Nicole Radde, Tim Ricken</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Frontiers in Physiology</t>
         </is>
       </c>
       <c r="D2" s="2" t="n">
@@ -5224,15 +5207,19 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>Organization Minisymposium</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>Computational Continuum Biomechanics</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>Tim Ricken, Oliver Röhrle, Silvia Budday</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr"/>
       <c r="D3" s="2" t="n">
         <v>44773</v>
       </c>
@@ -5250,15 +5237,19 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>Organization Minisymposium</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>CONTINUUM BIOMECHANICS OF ACTIVE SYSTEMS</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>Tim Ricken, Oliver Röhrle, Silvia Budday</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
       <c r="D4" s="2" t="n">
         <v>44717</v>
       </c>
@@ -5276,17 +5267,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>Editoring</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>Frontiers Research Topic “Multiscale Modeling for the Liver”</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>Ho H, Rezaina V, Schwen LO</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>https://www.frontiersin.org/research-topics/28431/multiscale-modeling-for-the-liver</t>
         </is>
       </c>
       <c r="D5" s="2" t="n">
@@ -5306,16 +5297,19 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Computational biomechanics and biomedical engineering of active
-biological systems – from methods to clinical application</t>
+          <t>Organization Minisymposium</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>Computational biomechanics and biomedical engineering of active biological systems – from methods to clinical application</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
           <t>Christian Bleiler, Lena Lambers, Renate Sachse</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr"/>
       <c r="D6" s="2" t="n">
         <v>44825</v>
       </c>
@@ -5333,17 +5327,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>Editoring</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t xml:space="preserve">Progress in Liver Stem Cell Therapy </t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t xml:space="preserve">Christ B, Oertel M </t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">MDPI </t>
         </is>
       </c>
       <c r="D7" s="2" t="n">
@@ -5363,15 +5357,19 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>Accepted project proposal</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t xml:space="preserve">Michael Stifel grant </t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t xml:space="preserve">Lena Lambers, Uta Dahmen </t>
         </is>
       </c>
-      <c r="C8" t="inlineStr"/>
       <c r="D8" s="2" t="n">
         <v>44712</v>
       </c>
@@ -5389,15 +5387,19 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t xml:space="preserve">Workshop </t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
           <t>Workshop on Computational Models in Biology and Medicine</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t xml:space="preserve">Nicole Radde, Sebastian Höpfl </t>
         </is>
       </c>
-      <c r="C9" t="inlineStr"/>
       <c r="D9" s="2" t="n">
         <v>44736</v>
       </c>
@@ -5415,15 +5417,19 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>Miscellaneous</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
           <t>Kongresssekretär der Jahrestagung der mittelseutschen Viszeralmedizin</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>Hans-Michael Tautenhahn</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
           <t>6/10/0022</t>
@@ -5443,15 +5449,19 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>Miscellaneous</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
           <t xml:space="preserve"> Vorstandsmitglied der Thüringischen Gesellschaft für Chirurgie</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>Hans-Michael Tautenhahn</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr">
         <is>
           <t>6/1/0022</t>
@@ -5471,15 +5481,19 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>Miscellaneous</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
           <t>New Project Assistant</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>Hans-Michael Tautenhahn</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr">
         <is>
           <t>8/1/0022</t>
@@ -5499,15 +5513,19 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t xml:space="preserve">Workshop Leader </t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
           <t>GmdS/IBS Arbeitsgruppe Mathematical Models in Medicine and Biology</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t xml:space="preserve">Nicole Radde, Ingmar Glauche </t>
         </is>
       </c>
-      <c r="C13" t="inlineStr"/>
       <c r="D13" s="2" t="n">
         <v>44760</v>
       </c>
@@ -5525,17 +5543,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>Accepted project proposal</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
           <t>Methodology for the calibration and analysis of stochastic models for heterogeneous intracellular processes with applications in cancer development</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>Nicole Radde</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>EXC 2075 - SimTech</t>
         </is>
       </c>
       <c r="D14" s="2" t="n">
@@ -5555,17 +5573,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>Accepted project proposal</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
           <t>Data-enhanced prediction of organ-specific tumor growth in the liver - a hybrid knowledge and data-driven approach</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>Tim Ricken</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>EXC 2075 - SimTech</t>
         </is>
       </c>
       <c r="D15" s="2" t="n">
@@ -5585,17 +5603,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
+          <t>Editoring</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
           <t>Editor-in-Chief der Zeitschrift "Zeitschrift für Medizinische Physik" (Journal of Medical Physics) (ISSN 0939-3889)</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="C16" t="inlineStr">
         <is>
           <t>Jürgen Reichenbach</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>"Zeitschrift für Medizinische Physik" (Journal of Medical Physics) (ISSN 0939-3889)</t>
         </is>
       </c>
       <c r="D16" s="2" t="n">
@@ -5615,15 +5633,19 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
+          <t>Internship</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
           <t>Computational Modeling of Drug Detoxification – A Systems Medicine Approach</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="C17" t="inlineStr">
         <is>
           <t>Matthias König</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr"/>
       <c r="D17" s="2" t="n">
         <v>44858</v>
       </c>
@@ -5641,15 +5663,19 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>Accepted project proposal</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
           <t xml:space="preserve">SIMulation supported LIVer Assessment for donor organs (SimLivA) - Continuum-biomechanical modeling for staging of ischemia reperfusion injury during liver transplantation </t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="C18" t="inlineStr">
         <is>
           <t>Professorin Dr. Uta Dahmen, Professor Dr.-Ing. Tim Ricken, Privatdozent Dr. Hans-Michael Tautenhahn, Dr. Matthias König</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr"/>
       <c r="D18" s="2" t="n">
         <v>44181</v>
       </c>
@@ -5667,16 +5693,19 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t xml:space="preserve">031L0304X - CompLS - Runde 5 -
-Verbundprojekt: ATLAS - Al and Simulation for Tumor Liver Assessment - Entwicklung eines Systems zur klinischen Entscheidungsunterstützung in der Diagnose und Behandlung von Lebertumoren auf Basis von künstlicher Intelligenz und Simulationen </t>
+          <t>Accepted project proposal</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
+          <t xml:space="preserve">031L0304X - CompLS - Runde 5 - Verbundprojekt: ATLAS - Al and Simulation for Tumor Liver Assessment - Entwicklung eines Systems zur klinischen Entscheidungsunterstützung in der Diagnose und Behandlung von Lebertumoren auf Basis von künstlicher Intelligenz und Simulationen </t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
           <t>Professor Dr.-Ing. Tim Ricken, Professor Dr. Steffen Staab, Privatdozent Dr. Hans-Michael Tautenhahn, Dr. Matthias König</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr"/>
       <c r="D19" s="2" t="n">
         <v>44819</v>
       </c>
@@ -5694,17 +5723,17 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
+          <t>Editoring</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
           <t>Elected PEtab editor from March 2023 until March 2026</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="C20" t="inlineStr">
         <is>
           <t>König Matthias</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>https://petab.readthedocs.io/en/latest/index.html</t>
         </is>
       </c>
       <c r="D20" s="2" t="n">
@@ -5724,15 +5753,19 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
+          <t>Accepted project proposal</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
           <t>X-Research Group: Physiologically based digital twins for the treatment of hypertension with ACE inhibitors and diuretics</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="C21" t="inlineStr">
         <is>
           <t>König Matthias</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr"/>
       <c r="D21" s="2" t="n">
         <v>44969</v>
       </c>
@@ -5750,15 +5783,19 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
+          <t>Editoring</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
           <t>M. König has been elected as PEtab editor (2023-2026)</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="C22" t="inlineStr">
         <is>
           <t>König Matthias</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr"/>
       <c r="D22" s="2" t="n">
         <v>44964</v>
       </c>
@@ -5776,17 +5813,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
           <t>Datasets for "Automated Detection of Portal Fields and Central Veins in Whole-Slide Images of Liver Tissue"</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="C23" t="inlineStr">
         <is>
           <t>Budelmann D, Laue H, Weis N, Dahmen U, D’Alessandro LA, Biermayer I, Klingmüller U, Ghallab A, Hassan R, Begher-Tibbe B, Hengstler JG, Schwen LO</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Zenodo 2022, doi: 10.5281/zenodo.5726769</t>
         </is>
       </c>
       <c r="D23" s="2" t="n">
@@ -5806,17 +5843,17 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
           <t>Dataset for "Segmentation of Lipid Droplets in Histological Images"</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="C24" t="inlineStr">
         <is>
           <t>Budelmann D, Cao Q, Laue H, Albadry M, Dahmen U, Schwen LO</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Zenodo 2023, doi: 10.5281/zenodo.7802211</t>
         </is>
       </c>
       <c r="D24" s="2" t="n">
@@ -5836,15 +5873,19 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
+          <t>Hosting and organization of COMBINE 2024</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
           <t>Hosting and organiztion of the Computational Modeling in Biology” Network (COMBINE) meeting 2024 in Stuttgart</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
+      <c r="C25" t="inlineStr">
         <is>
           <t>Radde Nicole, Waltemath Dagmar, Höpfl Sebastian</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr"/>
       <c r="D25" s="2" t="n">
         <v>45300</v>
       </c>
@@ -5862,15 +5903,19 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
+          <t>Organization Minisymposium</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
           <t>In-silico Models of Coupled Biological Systems</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
+      <c r="C26" t="inlineStr">
         <is>
           <t>Radde Nicole</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr"/>
       <c r="D26" s="2" t="n">
         <v>45056</v>
       </c>
@@ -5888,15 +5933,19 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
+          <t>Invited Speaker</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
           <t>Mathematische Modellbildung des Ischämie-Reperfusionsschadens zur Entscheidungsunterstützung bei Lebertransplantationen</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
+      <c r="C27" t="inlineStr">
         <is>
           <t>Mandl L., Gerhäusser S., Lambers L., König M., Tautenhahn H.-M., Dahmen U., Ricken T.</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr"/>
       <c r="D27" t="inlineStr">
         <is>
           <t>10/28/2023</t>

</xml_diff>

<commit_message>
minor fixes in tables
</commit_message>
<xml_diff>
--- a/assets/news/results/qualiperf_statistics.xlsx
+++ b/assets/news/results/qualiperf_statistics.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,135 +447,123 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>type</t>
+          <t>Asset</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>count</t>
+          <t>Count</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>qualiperf acknowledged</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>qualiperf not acknowledged</t>
+          <t>Qualiperf acknowledged</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>publications</t>
+          <t>Publications</t>
         </is>
       </c>
       <c r="B2" t="n">
         <v>33</v>
       </c>
-      <c r="C2" t="n">
-        <v>22</v>
-      </c>
-      <c r="D2" t="n">
-        <v>11</v>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>22 (66.7 %)</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>preprints</t>
+          <t>Preprints</t>
         </is>
       </c>
       <c r="B3" t="n">
         <v>9</v>
       </c>
-      <c r="C3" t="n">
-        <v>7</v>
-      </c>
-      <c r="D3" t="n">
-        <v>2</v>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>7 (77.8 %)</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>submissions</t>
+          <t>Submissions</t>
         </is>
       </c>
       <c r="B4" t="n">
         <v>2</v>
       </c>
-      <c r="C4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1</v>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>1 (50.0 %)</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>theses</t>
+          <t>Theses</t>
         </is>
       </c>
       <c r="B5" t="n">
         <v>5</v>
       </c>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" t="n">
-        <v>5</v>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0 (0.0 %)</t>
+        </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>posters</t>
+          <t>Posters</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>21</v>
       </c>
-      <c r="C6" t="n">
-        <v>19</v>
-      </c>
-      <c r="D6" t="n">
-        <v>2</v>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>19 (90.5 %)</t>
+        </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>presentations</t>
+          <t>Presentations</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>33</v>
       </c>
-      <c r="C7" t="n">
-        <v>26</v>
-      </c>
-      <c r="D7" t="n">
-        <v>7</v>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>26 (78.8 %)</t>
+        </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>others</t>
+          <t>Others</t>
         </is>
       </c>
       <c r="B8" t="n">
         <v>26</v>
       </c>
-      <c r="C8" t="n">
-        <v>4</v>
-      </c>
-      <c r="D8" t="n">
-        <v>22</v>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>4 (15.4 %)</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -696,7 +684,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 10.1515/jib-2021-0020</t>
+          <t>&lt;a href="https://doi.org/ 10.1515/jib-2021-0020"&gt; 10.1515/jib-2021-0020&lt;/a&gt;</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -747,7 +735,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>10.1515/jib-2021-0021</t>
+          <t>&lt;a href="https://doi.org/10.1515/jib-2021-0021"&gt;10.1515/jib-2021-0021&lt;/a&gt;</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -798,7 +786,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>10.3389/fphys.2021.733393</t>
+          <t>&lt;a href="https://doi.org/10.3389/fphys.2021.733393"&gt;10.3389/fphys.2021.733393&lt;/a&gt;</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -847,7 +835,7 @@
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr">
         <is>
-          <t xml:space="preserve">10.1007/s00419-021-01907-3 </t>
+          <t>&lt;a href="https://doi.org/10.1007/s00419-021-01907-3 "&gt;10.1007/s00419-021-01907-3 &lt;/a&gt;</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -898,7 +886,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 10.3389/fphys.2021.733868</t>
+          <t>&lt;a href="https://doi.org/ 10.3389/fphys.2021.733868"&gt; 10.3389/fphys.2021.733868&lt;/a&gt;</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -949,7 +937,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 10.1038/s41536-021-00194-4</t>
+          <t>&lt;a href="https://doi.org/ 10.1038/s41536-021-00194-4"&gt; 10.1038/s41536-021-00194-4&lt;/a&gt;</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -998,7 +986,7 @@
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr">
         <is>
-          <t>10.1002/pamm.202100190</t>
+          <t>&lt;a href="https://doi.org/10.1002/pamm.202100190"&gt;10.1002/pamm.202100190&lt;/a&gt;</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -1049,7 +1037,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>10.1038/s41392-021-00850-7</t>
+          <t>&lt;a href="https://doi.org/10.1038/s41392-021-00850-7"&gt;10.1038/s41392-021-00850-7&lt;/a&gt;</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -1098,7 +1086,7 @@
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr">
         <is>
-          <t>10.1016/j.ijsolstr.2021.111412</t>
+          <t>&lt;a href="https://doi.org/10.1016/j.ijsolstr.2021.111412"&gt;10.1016/j.ijsolstr.2021.111412&lt;/a&gt;</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -1149,7 +1137,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>10.3390/metabo12040293</t>
+          <t>&lt;a href="https://doi.org/10.3390/metabo12040293"&gt;10.3390/metabo12040293&lt;/a&gt;</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -1200,7 +1188,7 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>10.1515/jib-2021-0026</t>
+          <t>&lt;a href="https://doi.org/10.1515/jib-2021-0026"&gt;10.1515/jib-2021-0026&lt;/a&gt;</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -1251,7 +1239,7 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>10.3389/fphys.2022.859522</t>
+          <t>&lt;a href="https://doi.org/10.3389/fphys.2022.859522"&gt;10.3389/fphys.2022.859522&lt;/a&gt;</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
@@ -1268,9 +1256,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Tim Ricken, Lena Lambers, Bruno Christ, Uta Dahmen, Karl-Heinz Herrmann, Matthias
-König, Manja Marz, Nicole Radde, Jürgen R. Reichenbach, Lars Ole Schwen, and
-Hans-Michael Tautenhahn</t>
+          <t>Tim Ricken, Lena Lambers, Bruno Christ, Uta Dahmen, Karl-Heinz Herrmann, Matthias König, Manja Marz, Nicole Radde, Jürgen R. Reichenbach, Lars Ole Schwen, and Hans-Michael Tautenhahn</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1304,7 +1290,7 @@
       <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>&lt;a href="https://doi.org/-"&gt;-&lt;/a&gt;</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1355,7 +1341,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>10.3390/ijms23094564</t>
+          <t>&lt;a href="https://doi.org/10.3390/ijms23094564"&gt;10.3390/ijms23094564&lt;/a&gt;</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -1372,7 +1358,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Shaikh B, Smith LP, Vasilescu D, Marupilla G, Wilson M, Agmon E, Agnew H, Andrews SS, Anwar A, Beber ME, Bergmann FT, Brooks D, Brusch L, Calzone L, Choi K, Cooper J, Detloff J, Drawert B, Dumontier M, Ermentrout GB, Faeder JR, Freiburger AP, Fröhlich F, Funahashi A, Garny A, Gennari JH, Gleeson P, Goelzer A, Haiman Z, Hasenauer J, Hellerstein JL, Hermjakob H, Hoops S, Ison JC, Jahn D, Jakubowski HV, Jordan R, Kalaš M, &lt;b&gt;König M&lt;/b&gt;, Liebermeister W, Sheriff RSM, Mandal S, McDougal R, Medley JK, Mendes P, Müller R, Myers CJ, Naldi A, Nguyen TVN, Nickerson DP, Olivier BG, Patoliya D, Paulevé L, Petzold LR, Priya A, Rampadarath AK, Rohwer JM, Saglam AS, Singh D, Sinha A, Snoep J, Sorby H, Spangler R, Starruß J, Thomas PJ, van Niekerk D, Weindl D, Zhang F, Zhukova A, Goldberg AP, Schaff JC, Blinov ML, Sauro HM, Moraru II, Karr JR.</t>
+          <t>Shaikh B, Smith LP, Vasilescu D, Marupilla G, Wilson M, Agmon E, Agnew H, Andrews SS, Anwar A, Beber ME, Bergmann FT, Brooks D, Brusch L, Calzone L, Choi K, Cooper J, Detloff J, Drawert B, Dumontier M, Ermentrout GB, Faeder JR, Freiburger AP, Fröhlich F, Funahashi A, Garny A, Gennari JH, Gleeson P, Goelzer A, Haiman Z, Hasenauer J, Hellerstein JL, Hermjakob H, Hoops S, Ison JC, Jahn D, Jakubowski HV, Jordan R, Kalaš M, König M, Liebermeister W, Sheriff RSM, Mandal S, McDougal R, Medley JK, Mendes P, Müller R, Myers CJ, Naldi A, Nguyen TVN, Nickerson DP, Olivier BG, Patoliya D, Paulevé L, Petzold LR, Priya A, Rampadarath AK, Rohwer JM, Saglam AS, Singh D, Sinha A, Snoep J, Sorby H, Spangler R, Starruß J, Thomas PJ, van Niekerk D, Weindl D, Zhang F, Zhukova A, Goldberg AP, Schaff JC, Blinov ML, Sauro HM, Moraru II, Karr JR.</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1406,7 +1392,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>10.1093/nar/gkac331</t>
+          <t>&lt;a href="https://doi.org/10.1093/nar/gkac331"&gt;10.1093/nar/gkac331&lt;/a&gt;</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -1423,8 +1409,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Sandra Nickel, Madlen Christ, Sandra Schmidt, Joanna Kosacka, Hagen Kühne, Martin Roderfeld,
-Thomas Longerich, Lysann Tietze, Ina Bosse, Mei‐Ju Hsu, Peggy Stock, Elke Roeb, Bruno Christ</t>
+          <t>Sandra Nickel, Madlen Christ, Sandra Schmidt, Joanna Kosacka, Hagen Kühne, Martin Roderfeld, Thomas Longerich, Lysann Tietze, Ina Bosse, Mei‐Ju Hsu, Peggy Stock, Elke Roeb, Bruno Christ</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1458,7 +1443,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>10.3390/cells11111829</t>
+          <t>&lt;a href="https://doi.org/10.3390/cells11111829"&gt;10.3390/cells11111829&lt;/a&gt;</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -1509,7 +1494,7 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 10.1021/acssynbio.2c00118</t>
+          <t>&lt;a href="https://doi.org/ 10.1021/acssynbio.2c00118"&gt; 10.1021/acssynbio.2c00118&lt;/a&gt;</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
@@ -1558,7 +1543,7 @@
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr">
         <is>
-          <t>10.1016/j.ifacol.2023.01.020</t>
+          <t>&lt;a href="https://doi.org/10.1016/j.ifacol.2023.01.020"&gt;10.1016/j.ifacol.2023.01.020&lt;/a&gt;</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
@@ -1609,7 +1594,7 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>10.1007/s00104-022-01665-0</t>
+          <t>&lt;a href="https://doi.org/10.1007/s00104-022-01665-0"&gt;10.1007/s00104-022-01665-0&lt;/a&gt;</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
@@ -1660,7 +1645,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 10.1093/bioinformatics/btac501</t>
+          <t>&lt;a href="https://doi.org/ 10.1093/bioinformatics/btac501"&gt; 10.1093/bioinformatics/btac501&lt;/a&gt;</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -1709,7 +1694,7 @@
       <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr">
         <is>
-          <t>10.1016/j.exco.2022.100087</t>
+          <t>&lt;a href="https://doi.org/10.1016/j.exco.2022.100087"&gt;10.1016/j.exco.2022.100087&lt;/a&gt;</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -1760,7 +1745,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>10.1093/bioinformatics/btac770</t>
+          <t>&lt;a href="https://doi.org/10.1093/bioinformatics/btac770"&gt;10.1093/bioinformatics/btac770&lt;/a&gt;</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -1811,7 +1796,7 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>10.1038/s41598-022-26483-6</t>
+          <t>&lt;a href="https://doi.org/10.1038/s41598-022-26483-6"&gt;10.1038/s41598-022-26483-6&lt;/a&gt;</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
@@ -1828,8 +1813,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>S. M. Seyedpour, C. Henning, P. Kirmizakis, S. Herbrandt, K. Ickstadt, R. Doherty
-and T. Ricken</t>
+          <t>S. M. Seyedpour, C. Henning, P. Kirmizakis, S. Herbrandt, K. Ickstadt, R. Doherty and T. Ricken</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1861,7 +1845,7 @@
       <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr">
         <is>
-          <t>10.3390/w15010159</t>
+          <t>&lt;a href="https://doi.org/10.3390/w15010159"&gt;10.3390/w15010159&lt;/a&gt;</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -1910,7 +1894,7 @@
       <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr">
         <is>
-          <t>10.3390/w15020343</t>
+          <t>&lt;a href="https://doi.org/10.3390/w15020343"&gt;10.3390/w15020343&lt;/a&gt;</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -1961,7 +1945,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>10.1038/s41598-023-29340-2</t>
+          <t>&lt;a href="https://doi.org/10.1038/s41598-023-29340-2"&gt;10.1038/s41598-023-29340-2&lt;/a&gt;</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -2012,7 +1996,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 10.12659/AOT.938132</t>
+          <t>&lt;a href="https://doi.org/ 10.12659/AOT.938132"&gt; 10.12659/AOT.938132&lt;/a&gt;</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -2063,7 +2047,7 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>10.1515/jib-2023-0004</t>
+          <t>&lt;a href="https://doi.org/10.1515/jib-2023-0004"&gt;10.1515/jib-2023-0004&lt;/a&gt;</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
@@ -2114,7 +2098,7 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t xml:space="preserve">10.3389/fbioe.2023.1179980 </t>
+          <t>&lt;a href="https://doi.org/10.3389/fbioe.2023.1179980 "&gt;10.3389/fbioe.2023.1179980 &lt;/a&gt;</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
@@ -2165,7 +2149,7 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>10.1016/j.jpi.2022.100001</t>
+          <t>&lt;a href="https://doi.org/10.1016/j.jpi.2022.100001"&gt;10.1016/j.jpi.2022.100001&lt;/a&gt;</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
@@ -2216,7 +2200,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>10.1002/jmri.28698</t>
+          <t>&lt;a href="https://doi.org/10.1002/jmri.28698"&gt;10.1002/jmri.28698&lt;/a&gt;</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -2267,7 +2251,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t xml:space="preserve">10.3389/fendo.2023.1185656 </t>
+          <t>&lt;a href="https://doi.org/10.3389/fendo.2023.1185656 "&gt;10.3389/fendo.2023.1185656 &lt;/a&gt;</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -2318,7 +2302,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t xml:space="preserve">10.1038/s41598-023-42141-x </t>
+          <t>&lt;a href="https://doi.org/10.1038/s41598-023-42141-x "&gt;10.1038/s41598-023-42141-x &lt;/a&gt;</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
@@ -2430,7 +2414,7 @@
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
-          <t>10.20944/preprints202108.0303.v1</t>
+          <t>&lt;a href="https://doi.org/10.20944/preprints202108.0303.v1"&gt;10.20944/preprints202108.0303.v1&lt;/a&gt;</t>
         </is>
       </c>
     </row>
@@ -2471,7 +2455,7 @@
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr">
         <is>
-          <t>10.48550/arXiv.2106.00844</t>
+          <t>&lt;a href="https://doi.org/10.48550/arXiv.2106.00844"&gt;10.48550/arXiv.2106.00844&lt;/a&gt;</t>
         </is>
       </c>
     </row>
@@ -2483,8 +2467,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Matthias König* , Leandro H. Watanabe, Jan Grzegorzewski, Chris J.
-Myers</t>
+          <t>Matthias König* , Leandro H. Watanabe, Jan Grzegorzewski, Chris J. Myers</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2513,7 +2496,7 @@
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr">
         <is>
-          <t>10.1101/245076</t>
+          <t>&lt;a href="https://doi.org/10.1101/245076"&gt;10.1101/245076&lt;/a&gt;</t>
         </is>
       </c>
     </row>
@@ -2554,7 +2537,7 @@
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr">
         <is>
-          <t>10.20944/preprints202206.0137.v1</t>
+          <t>&lt;a href="https://doi.org/10.20944/preprints202206.0137.v1"&gt;10.20944/preprints202206.0137.v1&lt;/a&gt;</t>
         </is>
       </c>
     </row>
@@ -2595,7 +2578,7 @@
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr">
         <is>
-          <t>10.1101/2023.02.01.23285358</t>
+          <t>&lt;a href="https://doi.org/10.1101/2023.02.01.23285358"&gt;10.1101/2023.02.01.23285358&lt;/a&gt;</t>
         </is>
       </c>
     </row>
@@ -2607,7 +2590,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Mihail Anton, Eivind Almaas, Rui Benfeitas, Sara Benito-Vaquerizo, Lars M. Blank, Andreas Dräger, John M. Hancock, Cheewin Kittikunapong, &lt;b&gt;Matthias König&lt;/b&gt;, Feiran Li, Ulf W. Liebal, Hongzhong Lu, Hongwu Ma, Radhakrishnan Mahadevan, Adil Mardinoglu, Jens Nielsen, Juan Nogales, Marco Pagni, Jason A. Papin, Kiran Raosaheb Patil, Nathan D. Price, Jonathan L. Robinson, Benjamín J. Sánchez, Maria Suarez-Diez, Snorre Sulheim, L. Thomas Svensson, Bas Teusink, Wanwipa Vongsangnak, Hao Wang, Ahmad A. Zeidan, Eduard J. Kerkhoven</t>
+          <t>Mihail Anton, Eivind Almaas, Rui Benfeitas, Sara Benito-Vaquerizo, Lars M. Blank, Andreas Dräger, John M. Hancock, Cheewin Kittikunapong, Matthias König, Feiran Li, Ulf W. Liebal, Hongzhong Lu, Hongwu Ma, Radhakrishnan Mahadevan, Adil Mardinoglu, Jens Nielsen, Juan Nogales, Marco Pagni, Jason A. Papin, Kiran Raosaheb Patil, Nathan D. Price, Jonathan L. Robinson, Benjamín J. Sánchez, Maria Suarez-Diez, Snorre Sulheim, L. Thomas Svensson, Bas Teusink, Wanwipa Vongsangnak, Hao Wang, Ahmad A. Zeidan, Eduard J. Kerkhoven</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2636,7 +2619,7 @@
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr">
         <is>
-          <t>10.1101/2023.03.21.512712</t>
+          <t>&lt;a href="https://doi.org/10.1101/2023.03.21.512712"&gt;10.1101/2023.03.21.512712&lt;/a&gt;</t>
         </is>
       </c>
     </row>
@@ -2656,10 +2639,8 @@
           <t>bioRxiv 2023.04.12.536571; doi: https://doi.org/10.1101/2023.04.12.536571</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>4/14/2023</t>
-        </is>
+      <c r="D8" s="2" t="n">
+        <v>45030</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -2679,7 +2660,7 @@
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr">
         <is>
-          <t>10.1101/2023.04.12.536571</t>
+          <t>&lt;a href="https://doi.org/10.1101/2023.04.12.536571"&gt;10.1101/2023.04.12.536571&lt;/a&gt;</t>
         </is>
       </c>
     </row>
@@ -2699,10 +2680,8 @@
           <t>osfpreprints 2023.04.12.536571 doi: 10.31219/osf.io/kcvra</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>5/28/2023</t>
-        </is>
+      <c r="D9" s="2" t="n">
+        <v>45074</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -2722,7 +2701,7 @@
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr">
         <is>
-          <t>10.31219/osf.io/kcvra</t>
+          <t>&lt;a href="https://doi.org/10.31219/osf.io/kcvra"&gt;10.31219/osf.io/kcvra&lt;/a&gt;</t>
         </is>
       </c>
     </row>
@@ -2763,7 +2742,7 @@
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr">
         <is>
-          <t>10.21203/rs.3.rs-3348101/v1</t>
+          <t>&lt;a href="https://doi.org/10.21203/rs.3.rs-3348101/v1"&gt;10.21203/rs.3.rs-3348101/v1&lt;/a&gt;</t>
         </is>
       </c>
     </row>
@@ -3031,10 +3010,8 @@
           <t>Lambers, Lena</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>3/21/2023</t>
-        </is>
+      <c r="D4" s="2" t="n">
+        <v>45006</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -3068,10 +3045,8 @@
           <t>Beatrice Stemmer Mallol, Matthias König (supervisor)</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>7/17/2023</t>
-        </is>
+      <c r="D5" s="2" t="n">
+        <v>45124</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -3336,10 +3311,8 @@
           <t>SimTech Status Seminar 2022, Bad Boll</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>7/5/0022</t>
-        </is>
+      <c r="D6" s="2" t="n">
+        <v>44747</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -3688,10 +3661,8 @@
           <t>EASL European Association for the Study of the Liver, https://www.easlcongress.eu,</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>6/24/2023</t>
-        </is>
+      <c r="D16" s="2" t="n">
+        <v>45101</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -3725,10 +3696,8 @@
           <t>33., Wilseder Workshop von Biotest- Individulaisierte Therapie von Lebererkrnakungen, https://www.biotest-wilsede.de,</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>6/28/2023</t>
-        </is>
+      <c r="D17" s="2" t="n">
+        <v>45105</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -3762,10 +3731,8 @@
           <t>Workshop on Computational Models in Biology and Medicine 2023</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>6/15/2023</t>
-        </is>
+      <c r="D18" s="2" t="n">
+        <v>45092</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -3826,8 +3793,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t xml:space="preserve">Wan-Ting Zhao, Karl-Heinz Herrmann, Jürgen R. Reichenbach and Verena Hoerr
-</t>
+          <t xml:space="preserve">Wan-Ting Zhao, Karl-Heinz Herrmann, Jürgen R. Reichenbach and Verena Hoerr </t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -3853,13 +3819,27 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>39th European Society for Magnetic Resonance in Medicine and Biology, Basel, Switzerland. Poster</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
+          <t>39th European Society for Magnetic Resonance in Medicine and Biology, Basel, Switzerland. Poster LB280</t>
+        </is>
+      </c>
+      <c r="D21" s="2" t="n">
+        <v>45056</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Wan-Ting Zhao, Weiwei Wei, Karl-Heinz Herrmann, Uta Dahmen, Jürgen R. Reichenbach</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>P2 - Dahmen, P6 - Reichenbach</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -4136,8 +4116,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>15th World Congress on Computational Mechanics (WCCM-XV)
-8th Asian Pacific Congress on Computational Mechanics (APCOM-VIII)</t>
+          <t>15th World Congress on Computational Mechanics (WCCM-XV) 8th Asian Pacific Congress on Computational Mechanics (APCOM-VIII)</t>
         </is>
       </c>
       <c r="D7" s="2" t="n">
@@ -4175,10 +4154,8 @@
           <t>Jahrestagung der mitteldeutschen Viszeralmedizin</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>6/10/0022</t>
-        </is>
+      <c r="D8" s="2" t="n">
+        <v>44722</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -4239,8 +4216,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Lena Lambers, Steffen Gerhäusser, Luis Mandl, André Mielke
-and Tim Ricken</t>
+          <t>Lena Lambers, Steffen Gerhäusser, Luis Mandl, André Mielke and Tim Ricken</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -4388,10 +4364,8 @@
           <t>Combine Meeting, Satellite Event to the ICSB Conference, October 6-7, 2022, Berlin</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>10/6/0022</t>
-        </is>
+      <c r="D14" s="2" t="n">
+        <v>44840</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -4425,10 +4399,8 @@
           <t>3rd EnzymeML Workshop, October 18-19, 2022, Rüdesheim</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>10/18/0022</t>
-        </is>
+      <c r="D15" s="2" t="n">
+        <v>44852</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -4707,10 +4679,8 @@
           <t>MBM2023 - Workshop on Modelling in Biology and Medicine - https://mbm.systemsbiology.se</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>5/17/2023</t>
-        </is>
+      <c r="D23" s="2" t="n">
+        <v>45063</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -4744,10 +4714,8 @@
           <t>ISMB/ECCB 2023 Conference on Intelligent Systems for Molecular Biology (ISMB) and European Conference on Computational Biology (ECCB)</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>7/24/2023</t>
-        </is>
+      <c r="D24" s="2" t="n">
+        <v>45131</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -4816,10 +4784,8 @@
           <t>93. Jahrestagung der Gesellschaft für angewandte Mathematik und Mechanik (GAMM), Dresden</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>5/30/2023</t>
-        </is>
+      <c r="D26" s="2" t="n">
+        <v>45076</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -4853,10 +4819,8 @@
           <t>Workshop on Computational Models in Biology and Medicine 2023</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>6/16/2023</t>
-        </is>
+      <c r="D27" s="2" t="n">
+        <v>45093</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -4960,10 +4924,8 @@
           <t>X International Conference on Computational Bioengineering, Wien, 20.-22.09.2023, https://iccb2023.conf.tuwien.ac.at/</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>9/22/2023</t>
-        </is>
+      <c r="D30" s="2" t="n">
+        <v>45191</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -5032,10 +4994,8 @@
           <t>ICCB2023 - X International Conference on Computational Bioengineering</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>9/22/2023</t>
-        </is>
+      <c r="D32" s="2" t="n">
+        <v>45191</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -5430,10 +5390,8 @@
           <t>Hans-Michael Tautenhahn</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>6/10/0022</t>
-        </is>
+      <c r="D10" s="2" t="n">
+        <v>44722</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -5462,10 +5420,8 @@
           <t>Hans-Michael Tautenhahn</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>6/1/0022</t>
-        </is>
+      <c r="D11" s="2" t="n">
+        <v>44713</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -5494,10 +5450,8 @@
           <t>Hans-Michael Tautenhahn</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>8/1/0022</t>
-        </is>
+      <c r="D12" s="2" t="n">
+        <v>44774</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -5946,10 +5900,8 @@
           <t>Mandl L., Gerhäusser S., Lambers L., König M., Tautenhahn H.-M., Dahmen U., Ricken T.</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>10/28/2023</t>
-        </is>
+      <c r="D27" s="2" t="n">
+        <v>45227</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
fixing smaller issues in news
</commit_message>
<xml_diff>
--- a/assets/news/results/qualiperf_statistics.xlsx
+++ b/assets/news/results/qualiperf_statistics.xlsx
@@ -679,8 +679,10 @@
           <t>P3 - König</t>
         </is>
       </c>
-      <c r="I2" t="n">
-        <v>34668356</v>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>&lt;a href="https://pubmed.ncbi.nlm.nih.gov/34668356/"&gt;34668356&lt;/a&gt;</t>
+        </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -730,8 +732,10 @@
           <t>P3 - König</t>
         </is>
       </c>
-      <c r="I3" t="n">
-        <v>35330701</v>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>&lt;a href="https://pubmed.ncbi.nlm.nih.gov/35330701/"&gt;35330701&lt;/a&gt;</t>
+        </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -781,8 +785,10 @@
           <t>P9 - Tautenhahn</t>
         </is>
       </c>
-      <c r="I4" t="n">
-        <v>34630152</v>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>&lt;a href="https://pubmed.ncbi.nlm.nih.gov/34630152/"&gt;34630152&lt;/a&gt;</t>
+        </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -832,7 +838,11 @@
           <t>P6 - Reichenbach, P7 - Ricken, P9 - Tautenhahn, Coordination</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr"/>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>&lt;a href="https://pubmed.ncbi.nlm.nih.gov//"&gt;&lt;/a&gt;</t>
+        </is>
+      </c>
       <c r="J5" t="inlineStr">
         <is>
           <t>&lt;a href="https://doi.org/10.1007/s00419-021-01907-3 "&gt;10.1007/s00419-021-01907-3 &lt;/a&gt;</t>
@@ -881,8 +891,10 @@
           <t>P1 - Christ, P2 - Dahmen, P3 - König, P4 - Marz, P5 - Radde, P6 - Reichenbach, P7 - Ricken, P8 - Schwen, P9 - Tautenhahn, Coordination</t>
         </is>
       </c>
-      <c r="I6" t="n">
-        <v>34867441</v>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>&lt;a href="https://pubmed.ncbi.nlm.nih.gov/34867441/"&gt;34867441&lt;/a&gt;</t>
+        </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -932,8 +944,10 @@
           <t>P1 - Christ, P9 - Tautenhahn</t>
         </is>
       </c>
-      <c r="I7" t="n">
-        <v>34862411</v>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>&lt;a href="https://pubmed.ncbi.nlm.nih.gov/34862411/"&gt;34862411&lt;/a&gt;</t>
+        </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -983,7 +997,11 @@
           <t>P7 - Ricken, Coordination</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr"/>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>&lt;a href="https://pubmed.ncbi.nlm.nih.gov//"&gt;&lt;/a&gt;</t>
+        </is>
+      </c>
       <c r="J8" t="inlineStr">
         <is>
           <t>&lt;a href="https://doi.org/10.1002/pamm.202100190"&gt;10.1002/pamm.202100190&lt;/a&gt;</t>
@@ -1032,8 +1050,10 @@
           <t>P1 - Christ</t>
         </is>
       </c>
-      <c r="I9" t="n">
-        <v>34921132</v>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>&lt;a href="https://pubmed.ncbi.nlm.nih.gov/34921132/"&gt;34921132&lt;/a&gt;</t>
+        </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1083,7 +1103,11 @@
           <t>P7 - Ricken</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr"/>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>&lt;a href="https://pubmed.ncbi.nlm.nih.gov//"&gt;&lt;/a&gt;</t>
+        </is>
+      </c>
       <c r="J10" t="inlineStr">
         <is>
           <t>&lt;a href="https://doi.org/10.1016/j.ijsolstr.2021.111412"&gt;10.1016/j.ijsolstr.2021.111412&lt;/a&gt;</t>
@@ -1132,8 +1156,10 @@
           <t>P1 - Christ</t>
         </is>
       </c>
-      <c r="I11" t="n">
-        <v>35448480</v>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>&lt;a href="https://pubmed.ncbi.nlm.nih.gov/35448480/"&gt;35448480&lt;/a&gt;</t>
+        </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1183,8 +1209,10 @@
           <t>P3 - König</t>
         </is>
       </c>
-      <c r="I12" t="n">
-        <v>34674411</v>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>&lt;a href="https://pubmed.ncbi.nlm.nih.gov/34674411/"&gt;34674411&lt;/a&gt;</t>
+        </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1234,8 +1262,10 @@
           <t>P1 - Christ, P2 - Dahmen, P5 - Radde, P7 - Ricken</t>
         </is>
       </c>
-      <c r="I13" t="n">
-        <v>35242057</v>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>&lt;a href="https://pubmed.ncbi.nlm.nih.gov/35242057/"&gt;35242057&lt;/a&gt;</t>
+        </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1287,7 +1317,11 @@
           <t>P1 - Christ, P2 - Dahmen, P3 - König, P4 - Marz, P5 - Radde, P6 - Reichenbach, P7 - Ricken, P8 - Schwen, P9 - Tautenhahn, Coordination</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr"/>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>&lt;a href="https://pubmed.ncbi.nlm.nih.gov//"&gt;&lt;/a&gt;</t>
+        </is>
+      </c>
       <c r="J14" t="inlineStr">
         <is>
           <t>&lt;a href="https://doi.org/-"&gt;-&lt;/a&gt;</t>
@@ -1336,8 +1370,10 @@
           <t>P1 - Christ</t>
         </is>
       </c>
-      <c r="I15" t="n">
-        <v>35562954</v>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>&lt;a href="https://pubmed.ncbi.nlm.nih.gov/35562954/"&gt;35562954&lt;/a&gt;</t>
+        </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1387,8 +1423,10 @@
           <t>P3 - König</t>
         </is>
       </c>
-      <c r="I16" t="n">
-        <v>35524558</v>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>&lt;a href="https://pubmed.ncbi.nlm.nih.gov/35524558/"&gt;35524558&lt;/a&gt;</t>
+        </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1438,8 +1476,10 @@
           <t>P1 - Christ</t>
         </is>
       </c>
-      <c r="I17" t="n">
-        <v>35681524</v>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>&lt;a href="https://pubmed.ncbi.nlm.nih.gov/35681524/"&gt;35681524&lt;/a&gt;</t>
+        </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1489,8 +1529,10 @@
           <t>P5 - Radde</t>
         </is>
       </c>
-      <c r="I18" t="n">
-        <v>35749318</v>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>&lt;a href="https://pubmed.ncbi.nlm.nih.gov/35749318/"&gt;35749318&lt;/a&gt;</t>
+        </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1540,7 +1582,11 @@
           <t>P5 - Radde</t>
         </is>
       </c>
-      <c r="I19" t="inlineStr"/>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>&lt;a href="https://pubmed.ncbi.nlm.nih.gov//"&gt;&lt;/a&gt;</t>
+        </is>
+      </c>
       <c r="J19" t="inlineStr">
         <is>
           <t>&lt;a href="https://doi.org/10.1016/j.ifacol.2023.01.020"&gt;10.1016/j.ifacol.2023.01.020&lt;/a&gt;</t>
@@ -1589,8 +1635,10 @@
           <t>P9 - Tautenhahn</t>
         </is>
       </c>
-      <c r="I20" t="n">
-        <v>35771270</v>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>&lt;a href="https://pubmed.ncbi.nlm.nih.gov/35771270/"&gt;35771270&lt;/a&gt;</t>
+        </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1640,8 +1688,10 @@
           <t>P5 - Radde</t>
         </is>
       </c>
-      <c r="I21" t="n">
-        <v>35916726</v>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>&lt;a href="https://pubmed.ncbi.nlm.nih.gov/35916726/"&gt;35916726&lt;/a&gt;</t>
+        </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -1691,7 +1741,11 @@
           <t>P7 - Ricken</t>
         </is>
       </c>
-      <c r="I22" t="inlineStr"/>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>&lt;a href="https://pubmed.ncbi.nlm.nih.gov//"&gt;&lt;/a&gt;</t>
+        </is>
+      </c>
       <c r="J22" t="inlineStr">
         <is>
           <t>&lt;a href="https://doi.org/10.1016/j.exco.2022.100087"&gt;10.1016/j.exco.2022.100087&lt;/a&gt;</t>
@@ -1740,8 +1794,10 @@
           <t>P3 - König</t>
         </is>
       </c>
-      <c r="I23" t="n">
-        <v>36478036</v>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>&lt;a href="https://pubmed.ncbi.nlm.nih.gov/36478036/"&gt;36478036&lt;/a&gt;</t>
+        </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -1791,8 +1847,10 @@
           <t>P1 - Christ, P2 - Dahmen, P3 - König, P5 - Radde, P8 - Schwen</t>
         </is>
       </c>
-      <c r="I24" t="n">
-        <v>36528753</v>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>&lt;a href="https://pubmed.ncbi.nlm.nih.gov/36528753/"&gt;36528753&lt;/a&gt;</t>
+        </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -1842,7 +1900,11 @@
           <t>P7 - Ricken</t>
         </is>
       </c>
-      <c r="I25" t="inlineStr"/>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>&lt;a href="https://pubmed.ncbi.nlm.nih.gov//"&gt;&lt;/a&gt;</t>
+        </is>
+      </c>
       <c r="J25" t="inlineStr">
         <is>
           <t>&lt;a href="https://doi.org/10.3390/w15010159"&gt;10.3390/w15010159&lt;/a&gt;</t>
@@ -1891,7 +1953,11 @@
           <t>P7 - Ricken</t>
         </is>
       </c>
-      <c r="I26" t="inlineStr"/>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>&lt;a href="https://pubmed.ncbi.nlm.nih.gov//"&gt;&lt;/a&gt;</t>
+        </is>
+      </c>
       <c r="J26" t="inlineStr">
         <is>
           <t>&lt;a href="https://doi.org/10.3390/w15020343"&gt;10.3390/w15020343&lt;/a&gt;</t>
@@ -1940,8 +2006,10 @@
           <t>P5 - Radde</t>
         </is>
       </c>
-      <c r="I27" t="n">
-        <v>36792648</v>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>&lt;a href="https://pubmed.ncbi.nlm.nih.gov/36792648/"&gt;36792648&lt;/a&gt;</t>
+        </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -1991,8 +2059,10 @@
           <t>P9 - Tautenhahn</t>
         </is>
       </c>
-      <c r="I28" t="n">
-        <v>36927714</v>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>&lt;a href="https://pubmed.ncbi.nlm.nih.gov/36927714/"&gt;36927714&lt;/a&gt;</t>
+        </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -2042,8 +2112,10 @@
           <t>P3 - König</t>
         </is>
       </c>
-      <c r="I29" t="n">
-        <v>36989443</v>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>&lt;a href="https://pubmed.ncbi.nlm.nih.gov/36989443/"&gt;36989443&lt;/a&gt;</t>
+        </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -2093,8 +2165,10 @@
           <t>P8 - Schwen</t>
         </is>
       </c>
-      <c r="I30" t="n">
-        <v>37122862</v>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>&lt;a href="https://pubmed.ncbi.nlm.nih.gov/37122862/"&gt;37122862&lt;/a&gt;</t>
+        </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -2144,8 +2218,10 @@
           <t>Stea-PK Mod</t>
         </is>
       </c>
-      <c r="I31" t="n">
-        <v>35242441</v>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>&lt;a href="https://pubmed.ncbi.nlm.nih.gov/35242441/"&gt;35242441&lt;/a&gt;</t>
+        </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -2195,8 +2271,10 @@
           <t>P6 - Reichenbach</t>
         </is>
       </c>
-      <c r="I32" t="n">
-        <v>37026419</v>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>&lt;a href="https://pubmed.ncbi.nlm.nih.gov/37026419/"&gt;37026419&lt;/a&gt;</t>
+        </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -2246,8 +2324,10 @@
           <t>P3 - König</t>
         </is>
       </c>
-      <c r="I33" t="n">
-        <v>37600713</v>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>&lt;a href="https://pubmed.ncbi.nlm.nih.gov/37600713/"&gt;37600713&lt;/a&gt;</t>
+        </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -2297,8 +2377,10 @@
           <t>P7 - Ricken, SimLivA, ATLAS</t>
         </is>
       </c>
-      <c r="I34" t="n">
-        <v>37730743</v>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>&lt;a href="https://pubmed.ncbi.nlm.nih.gov/37730743/"&gt;37730743&lt;/a&gt;</t>
+        </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -2322,7 +2404,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2368,11 +2450,6 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Pubmed</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
           <t>DOI</t>
         </is>
       </c>
@@ -2411,8 +2488,7 @@
           <t>P3 - König</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>&lt;a href="https://doi.org/10.20944/preprints202108.0303.v1"&gt;10.20944/preprints202108.0303.v1&lt;/a&gt;</t>
         </is>
@@ -2452,8 +2528,7 @@
           <t>P3 - König</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>&lt;a href="https://doi.org/10.48550/arXiv.2106.00844"&gt;10.48550/arXiv.2106.00844&lt;/a&gt;</t>
         </is>
@@ -2493,8 +2568,7 @@
           <t>P3 - König</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>&lt;a href="https://doi.org/10.1101/245076"&gt;10.1101/245076&lt;/a&gt;</t>
         </is>
@@ -2534,8 +2608,7 @@
           <t>P3 - König</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>&lt;a href="https://doi.org/10.20944/preprints202206.0137.v1"&gt;10.20944/preprints202206.0137.v1&lt;/a&gt;</t>
         </is>
@@ -2575,8 +2648,7 @@
           <t>P3 - König, P9 - Tautenhahn</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>&lt;a href="https://doi.org/10.1101/2023.02.01.23285358"&gt;10.1101/2023.02.01.23285358&lt;/a&gt;</t>
         </is>
@@ -2616,8 +2688,7 @@
           <t>P3 - König</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t>&lt;a href="https://doi.org/10.1101/2023.03.21.512712"&gt;10.1101/2023.03.21.512712&lt;/a&gt;</t>
         </is>
@@ -2657,8 +2728,7 @@
           <t>P3 - König, P9 - Tautenhahn</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>&lt;a href="https://doi.org/10.1101/2023.04.12.536571"&gt;10.1101/2023.04.12.536571&lt;/a&gt;</t>
         </is>
@@ -2698,8 +2768,7 @@
           <t>P3 - König</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t>&lt;a href="https://doi.org/10.31219/osf.io/kcvra"&gt;10.31219/osf.io/kcvra&lt;/a&gt;</t>
         </is>
@@ -2739,8 +2808,7 @@
           <t>P2 - Dahmen, P3 - König, P7 - Ricken, P9 - Tautenhahn</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr">
+      <c r="H10" t="inlineStr">
         <is>
           <t>&lt;a href="https://doi.org/10.21203/rs.3.rs-3348101/v1"&gt;10.21203/rs.3.rs-3348101/v1&lt;/a&gt;</t>
         </is>
@@ -2757,7 +2825,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2778,25 +2846,20 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Journal</t>
+          <t>Date</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Date</t>
+          <t>Qualiperf</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Qualiperf</t>
+          <t>Authors Qualiperf</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Authors Qualiperf</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Projects</t>
         </is>
@@ -2813,25 +2876,20 @@
           <t xml:space="preserve">*Wagner Vincent, *Höpfl Sebastian, Klingel Viviane, Pop Maria C. , Radde Nicole E. </t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>IFAC-PapersOnline series, https://www.sciencedirect.com/journal/ifac-papersonline</t>
-        </is>
-      </c>
-      <c r="D2" s="2" t="n">
+      <c r="C2" s="2" t="n">
         <v>44664</v>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>Sebastian Höpfl, Nicole Erika Radde</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
-        <is>
-          <t>Sebastian Höpfl, Nicole Erika Radde</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
         <is>
           <t>P5 - Radde</t>
         </is>
@@ -2848,21 +2906,20 @@
           <t>Budelmann D, Cao Q, Laue H, Albadry M, Dahmen U, Schwen LO</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" s="2" t="n">
+      <c r="C3" s="2" t="n">
         <v>45081</v>
       </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>(None received QuaLiPerF funding for this work)</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
-        <is>
-          <t>(None received QuaLiPerF funding for this work)</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
         <is>
           <t>Stea-PK Mod</t>
         </is>

</xml_diff>

<commit_message>
first figures for the assets
</commit_message>
<xml_diff>
--- a/assets/news/results/qualiperf_statistics.xlsx
+++ b/assets/news/results/qualiperf_statistics.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,6 +460,16 @@
           <t>Qualiperf acknowledged</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -475,6 +485,12 @@
           <t>22 (66.7 %)</t>
         </is>
       </c>
+      <c r="D2" t="n">
+        <v>22</v>
+      </c>
+      <c r="E2" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -490,6 +506,12 @@
           <t>7 (77.8 %)</t>
         </is>
       </c>
+      <c r="D3" t="n">
+        <v>7</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -505,6 +527,12 @@
           <t>1 (50.0 %)</t>
         </is>
       </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -520,6 +548,12 @@
           <t>0 (0.0 %)</t>
         </is>
       </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -535,6 +569,12 @@
           <t>19 (90.5 %)</t>
         </is>
       </c>
+      <c r="D6" t="n">
+        <v>19</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -550,6 +590,12 @@
           <t>26 (78.8 %)</t>
         </is>
       </c>
+      <c r="D7" t="n">
+        <v>26</v>
+      </c>
+      <c r="E7" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -564,6 +610,12 @@
         <is>
           <t>4 (15.4 %)</t>
         </is>
+      </c>
+      <c r="D8" t="n">
+        <v>4</v>
+      </c>
+      <c r="E8" t="n">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>